<commit_message>
future reference ammo weight
</commit_message>
<xml_diff>
--- a/changes/545-mags.xlsx
+++ b/changes/545-mags.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yifan\Documents\deadline-balancing\changes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6752BC0-28FF-480F-BD0E-77C7CA6F393C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B5BED2A-BA7C-4A8C-97C5-86B953955B80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t>old</t>
   </si>
@@ -153,6 +153,9 @@
   </si>
   <si>
     <t>RPK 16 95R</t>
+  </si>
+  <si>
+    <t>ammo weight: 0.3703766</t>
   </si>
 </sst>
 </file>
@@ -427,7 +430,7 @@
   <dimension ref="A1:AE999"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AE5" sqref="AE5"/>
+      <selection activeCell="AH6" sqref="AH6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -474,7 +477,9 @@
         <v>2</v>
       </c>
       <c r="AD1" s="1"/>
-      <c r="AE1" s="1"/>
+      <c r="AE1" s="1" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="2" spans="1:31" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -1281,7 +1286,6 @@
         <v>0</v>
       </c>
       <c r="AB14" s="1"/>
-      <c r="AC14" s="1"/>
       <c r="AD14" s="1"/>
       <c r="AE14" s="1"/>
     </row>

</xml_diff>